<commit_message>
Writing to excel workbook
</commit_message>
<xml_diff>
--- a/11_word_excel/ITEC_Courses.xlsx
+++ b/11_word_excel/ITEC_Courses.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student1/Documents/1150ProgrammingLogic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student1/Development/python/ProgrammingLogic1150Examples/11_word_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91788BDC-66B9-1545-BBC8-C89AFEBA6A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4E1A5-59B9-6142-878C-7FAEDAD594A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="2340" windowWidth="19400" windowHeight="13520" xr2:uid="{39104375-FB91-B944-AFEC-2ADF1FFBC11E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="codes" sheetId="1" r:id="rId1"/>
+    <sheet name="rooms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>ITEC</t>
   </si>
@@ -49,6 +50,21 @@
   </si>
   <si>
     <t>Microsoft Windows Operating Systems</t>
+  </si>
+  <si>
+    <t>T-3010</t>
+  </si>
+  <si>
+    <t>T-3030</t>
+  </si>
+  <si>
+    <t>T-3050</t>
+  </si>
+  <si>
+    <t>T-3080</t>
+  </si>
+  <si>
+    <t>T-3020</t>
   </si>
 </sst>
 </file>
@@ -402,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D6A6D8-17A8-FB43-95F1-6ABCD328FB1C}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -488,4 +502,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E696B5-7179-7042-956F-43B5913BB7A4}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>